<commit_message>
NAICS data source refresh
</commit_message>
<xml_diff>
--- a/xls_files/2-6 digit_2017_Codes.xlsx
+++ b/xls_files/2-6 digit_2017_Codes.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z035330\Documents\JJAUSSI\Other\JC\projects\LDSBC\IT_243\repos\DFNB_dw_slvd\xls_files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4883B0B-EB90-45F1-91D9-D3C61633B110}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="3360" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15180" windowHeight="8070"/>
   </bookViews>
   <sheets>
     <sheet name="tbl_2017_title_description_coun" sheetId="1" r:id="rId1"/>
@@ -4990,7 +4984,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5104,8 +5098,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -5163,7 +5157,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5196,26 +5190,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5248,23 +5225,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5440,7 +5400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>